<commit_message>
[Abraham ]:Update file excel.
</commit_message>
<xml_diff>
--- a/src/assets/anexos/documento_cargar_monedas.xlsx
+++ b/src/assets/anexos/documento_cargar_monedas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/papamacone/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/papamactwo/Desktop/Project/MegaBahia/grp-front-center/src/assets/anexos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0418D61F-3321-B64C-9495-83E1B9DAA148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC58727B-4E64-2C41-B399-AE1DAD38C14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18620" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{3FDAB71D-9125-44FE-8F2C-4B501D5972E1}"/>
+    <workbookView xWindow="3140" yWindow="2280" windowWidth="23260" windowHeight="12580" xr2:uid="{3FDAB71D-9125-44FE-8F2C-4B501D5972E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Clientes" sheetId="1" r:id="rId1"/>
@@ -32,34 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
-  <si>
-    <t>identificacion</t>
-  </si>
-  <si>
-    <t>nombres</t>
-  </si>
-  <si>
-    <t>apellidos</t>
-  </si>
-  <si>
-    <t>ruc</t>
-  </si>
-  <si>
-    <t>empresa</t>
-  </si>
-  <si>
-    <t>monto</t>
-  </si>
-  <si>
-    <t>fecha asignacion</t>
-  </si>
-  <si>
-    <t>fecha vigencia</t>
-  </si>
-  <si>
-    <t>concepto</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>jimmy</t>
   </si>
@@ -79,9 +52,6 @@
     <t>2022-10-12</t>
   </si>
   <si>
-    <t>2022-12-31</t>
-  </si>
-  <si>
     <t>Joaquin</t>
   </si>
   <si>
@@ -94,12 +64,6 @@
     <t>2022-10-13</t>
   </si>
   <si>
-    <t>2023-01-10</t>
-  </si>
-  <si>
-    <t>Correo</t>
-  </si>
-  <si>
     <t>jimmy1817@hotmail.com</t>
   </si>
   <si>
@@ -107,13 +71,40 @@
   </si>
   <si>
     <t>0803236561</t>
+  </si>
+  <si>
+    <t>CÉDULA DEL EMPLEADO</t>
+  </si>
+  <si>
+    <t>NOMBRE DEL EMPLEADO</t>
+  </si>
+  <si>
+    <t>APELLIDO DEL EMPLEADO</t>
+  </si>
+  <si>
+    <t>CORREO DEL EMPLEADO</t>
+  </si>
+  <si>
+    <t>RUC DE LA EMPRESA QUE OTORGA BIG PUNTOS</t>
+  </si>
+  <si>
+    <t>NOMBRE DE LA EMPRESA</t>
+  </si>
+  <si>
+    <t>CANTIDAD DE BIG PUNTOS ASIGNADOS</t>
+  </si>
+  <si>
+    <t>FECHA DE ASIGNACIÓN</t>
+  </si>
+  <si>
+    <t>CONCEPTO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +122,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -157,10 +156,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -476,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13EB2F13-6A63-4DA8-9EC2-4477BE5BC753}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -490,104 +492,94 @@
     <col min="5" max="5" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="10.83203125" style="1"/>
     <col min="8" max="8" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+    <row r="1" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1003150602</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="G2" s="1">
         <v>300</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>